<commit_message>
Add today tests to Manuális_tesztek.xlsx
</commit_message>
<xml_diff>
--- a/documentation/Manuális_tesztek.xlsx
+++ b/documentation/Manuális_tesztek.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CZente\Desktop\shared\dev\nodejs\FoxHabits\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5E7028-4E2A-45E5-A1F7-27EFDC366822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CFC864-FF73-4ADE-92DD-565E3AA19F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Manuális tesztek" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="119">
   <si>
     <t>Leírás</t>
   </si>
@@ -201,76 +201,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tesztkörnyezet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Operációs rendszer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Mac OS 15.1
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Böngésző</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Google Chrome 131.0.6778.70, Safari 18.1</t>
-    </r>
-  </si>
-  <si>
     <t>1. Nyisd meg a regisztráció oldalt
 2. Írd be egy nevet, egy létező email címet, jelszót és a jelszó megerősítését
 3. Kattints a Regisztráció gombra.</t>
@@ -297,6 +227,875 @@
         <scheme val="minor"/>
       </rPr>
       <t>Lénárt Dániel Péter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. tesztelés (2024. 12. 06.)
+Tesztelő: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ceglédi Zente Holló</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tesztkörnyezet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Operációs rendszer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Mac OS 15.1
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Böngésző</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Google Chrome 131.0.6778.70, Safari 18.1
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Build</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 268e0ff (fox-habits.vercel.app)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tesztkörnyezet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Operációs rendszer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Microsoft Windows [Version 10.0.19045.5131]
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Böngésző</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Brave: 1.73.91 Chromium: 131.0.6778.85 (Hivatalos verzió) (64 bites) 
+- Build: 32998e9 (foxhabits.com)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tesztelt modulok/funkciók</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Bejelentkezés
+- Regisztráció</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Elfelejtett jelszó</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Nyisd meg a regisztráció oldalt.
+2. Adj meg érvényes nevet, e-mail címet, jelszót, és azonos jelszót a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jelszó megerősítése</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mezőbe
+3. Kattints a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Regisztráció</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gombra.</t>
+    </r>
+  </si>
+  <si>
+    <t>Regisztráció érvényes adatokkal, e-mail címmel</t>
+  </si>
+  <si>
+    <t>A rendszer átdobja a felhasználót a bejelentkezés oldalra. (regisztrálódik a felhasználó az adatbázisba)</t>
+  </si>
+  <si>
+    <t>B003</t>
+  </si>
+  <si>
+    <t>B002/1</t>
+  </si>
+  <si>
+    <t>B002/2</t>
+  </si>
+  <si>
+    <t>B002/3</t>
+  </si>
+  <si>
+    <t>E-mailt kell kapnod a visszaállítási linkkel.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pass
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Nincs formázva a visszaállító e-mail)</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Nyisd meg az elfelejtett jelszó oldalt.
+2. Add meg az e-mail címed
+3. Kattints a visszaállítási link küldése gombra.</t>
+  </si>
+  <si>
+    <t>1. Kattints az e-mailben kapott linkre
+2. Adj meg egy új jelszót és erősítsd meg.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Az oldalnak be kell jelentkeznie, és át kell dobnia a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>profil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> oldalra.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Nyisd meg a bejelentkezés oldalt.
+2. Jelentkezz be a megváltoztatott jelszóval.</t>
+  </si>
+  <si>
+    <t>Az oldalnak be kell jelentkeztetnie a felhasználót.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A rendszer bejelentkezik, a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>profil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> oldal megjelenik.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Partially
+Nem kapott értesítést a sikeres regisztrációról, vagy arról, hogy ellenőrző e-mailt küldtek. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ellenőrző mail nincs formázva)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Partially
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nincs olyan szigorú jelszó ellenőrzés, mint a létrehozásnál. Például elfogadott jelszó: "Admin12".
+Átdobás után nem frissül a header</t>
+    </r>
+  </si>
+  <si>
+    <t>B001/2</t>
+  </si>
+  <si>
+    <t>B001/1</t>
+  </si>
+  <si>
+    <t>Partially
+Jóváhagyásra kerül az e-mail, de nem kap értesítést a sikeres jóváhagyásról az oldalon.</t>
+  </si>
+  <si>
+    <t>1. Kattints az e-mailben kapott linkre.</t>
+  </si>
+  <si>
+    <t>Jóváhagyásra kerül az e-mail cím</t>
+  </si>
+  <si>
+    <t>B004/1</t>
+  </si>
+  <si>
+    <t>B004/2</t>
+  </si>
+  <si>
+    <t>B004/3</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>B005</t>
+  </si>
+  <si>
+    <t>Bejelentkezés Google-lel, még nem létező felhasználó esetén.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <t>Fail
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ismeretlen hiba. Próbálja újra.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+(megjegyzés: nem kapott a regisztrációt jóváhagyandó e-mailt)</t>
+    </r>
+  </si>
+  <si>
+    <t>Az SMTP hibák erre vezethetőek vissza:</t>
+  </si>
+  <si>
+    <t>Teszthez használt dummy adatok</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eredmény</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 100% (10/10)</t>
+    </r>
+  </si>
+  <si>
+    <t>Név: Kovács József 
+E-mail: kamuemail4@zente.org
+Jelszó: KovacsJozsi12!
+Jelszó megerősítése: KovacsJozsi12!</t>
+  </si>
+  <si>
+    <t>E-mail: cegledizente@gmail.com</t>
+  </si>
+  <si>
+    <t>E-mail: zentecegledi@gmail.com</t>
+  </si>
+  <si>
+    <t>B006</t>
+  </si>
+  <si>
+    <t>Jelszó visszaállítás kérése nem létező felhasználó esetében</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Nyisd meg a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jelszó visszaállítás</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> oldalt.
+2. Adj meg, egy az oldalon nem regisztrált e-mail címet.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hibaüzenet visszaadása</t>
+  </si>
+  <si>
+    <t>Jelszó: 111111, 11111111, Admin12, Admin12!, Admin123!, Admin123456!%/</t>
+  </si>
+  <si>
+    <t>Fail
+"Hiba történt a jelszó módosítása során"</t>
+  </si>
+  <si>
+    <t>B007</t>
+  </si>
+  <si>
+    <t>Jelszó visszaállítási linkre való kattintás másodszorra</t>
+  </si>
+  <si>
+    <t>1. Kattints másodjára is a jelszó visszaállítása e-mailben található linkre.</t>
+  </si>
+  <si>
+    <t>Fail
+Üzenet: "Jelszó visszaállítási link elküldve az alábbi e-mail címre."</t>
+  </si>
+  <si>
+    <t>E-mail: czh@czh.hu (nem regisztrált)</t>
+  </si>
+  <si>
+    <t>Hiba forrása/Lehetséges megoldás/Megjegyzés</t>
+  </si>
+  <si>
+    <t>E-mail (Google): zentehollo@gmail.com</t>
+  </si>
+  <si>
+    <t>Esetleg megcsinálhatnánk, hogy a bejelentkezés oldalról is elérhető legyen a Google belépés</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg a bejelentkezés oldalt.
+2. Kattints a Google-lel való belépés gombra
+3. Csináld végig a Google autentikációját</t>
+  </si>
+  <si>
+    <t>B008</t>
+  </si>
+  <si>
+    <t>Bejelentkezés Google-lel, már korábban e-mailel regisztrált felhasználó esetén.</t>
+  </si>
+  <si>
+    <t>B009</t>
+  </si>
+  <si>
+    <t>Bejelentkezés Google-lel, korábban már Google-lel regisztrált felhasználó esetén.</t>
+  </si>
+  <si>
+    <t>B010</t>
+  </si>
+  <si>
+    <t>Regisztráció, helytelen megerősítő jelszóval.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jelszó visszaállítás kérése, jelszó megváltoztatása majd bejelentkezés
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jelszó visszaállítás kérése, jelszó megváltoztatása majd bejelentkezés </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(2.)</t>
+    </r>
+  </si>
+  <si>
+    <t>Fail
+Nincs üzenet
+"https://www.foxhabits.com/auth/reset-password?error=access_denied&amp;error_code=403&amp;error_description=Email+link+is+invalid+or+has+expired#error=access_denied&amp;error_code=403&amp;error_description=Email+link+is+invalid+or+has+expired"</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg a bejelentkezés oldalt.
+2. Kattints a Google-lel való belépés gombra
+3. Csináld végig a Google autentikációját egy olyan fiókkal, amelyel már korábban regisztráltál a Google authentikációval.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A felhasználó átdobása a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>profil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> oldalra a bejelentkezett fiókkal.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jelszavak nem egyeznek</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hibaüzenetet kell visszaadnia</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Nyisd meg a regisztráció oldalt.
+2. Adj meg érvényes nevet, e-mail címet, jelszót és írj meg egy eltérő jelszót a jelszó megerősítése mezőbe.
+3. Kattints a Regisztráció gombra.</t>
+  </si>
+  <si>
+    <t>Név: CZH
+E-mail: cegledizentehollo@gmail.eu.admin
+Jelszó: Admin.123
+Jelszó megerősítése: Admin.124</t>
+  </si>
+  <si>
+    <t>1. Nyisd meg a bejelentkezés oldalt.
+2. Kattints a Google-lel való belépés gombra
+3. Csináld végig a Google autentikációját egy olyan fiókkal, amelyel már korábban regisztráltál e-mail címmel.</t>
+  </si>
+  <si>
+    <t>Nincs SMTP konfigurálva, Supabase limitálja az óránként kiküldhető e-mailek számát 2-re konfig nélkül</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eredmény</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 46.67% (7/15)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partially</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 20.00% (3/15)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 26.67% (4/15)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 6.67% (1/15)</t>
     </r>
   </si>
 </sst>
@@ -304,7 +1103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +1114,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -339,6 +1146,22 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -348,7 +1171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -400,6 +1223,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -469,13 +1307,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -488,8 +1339,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -501,8 +1354,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -514,8 +1369,10 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -524,10 +1381,19 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -545,7 +1411,27 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -554,10 +1440,51 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -569,7 +1496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -577,73 +1504,115 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -664,7 +1633,56 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -679,6 +1697,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9338</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>186765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>342450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1206082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99EEB0A6-9238-B753-1E14-A17C74CA7AF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10598897" y="9851839"/>
+          <a:ext cx="8830907" cy="1019317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>91587</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>424234</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>699299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40E14AA1-B497-A9C6-1060-12C63EC80C34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10065361" y="15926899"/>
+          <a:ext cx="7906853" cy="2219635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -944,10 +2055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="129" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,44 +2066,56 @@
     <col min="1" max="1" width="12.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="62.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="29.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="28" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1002,14 +2125,20 @@
       <c r="C3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G3" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1019,14 +2148,20 @@
       <c r="C4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G4" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1036,14 +2171,20 @@
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1053,14 +2194,20 @@
       <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G6" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1070,14 +2217,20 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G7" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1087,14 +2240,20 @@
       <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G8" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1104,14 +2263,20 @@
       <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G9" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -1121,14 +2286,20 @@
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G10" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -1136,52 +2307,459 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D12" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"Fail"</formula>
+  <conditionalFormatting sqref="F2:F13 F15:F1048576">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",F2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Pass"</formula>
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F13 F15:F1048576">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Skip">
+      <formula>NOT(ISERROR(SEARCH("Skip",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Partially">
+      <formula>NOT(ISERROR(SEARCH("Partially",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new tests (B1XX)
</commit_message>
<xml_diff>
--- a/documentation/Manuális_tesztek.xlsx
+++ b/documentation/Manuális_tesztek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CZente\Desktop\shared\dev\nodejs\FoxHabits\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2614929-139A-40D4-9B12-AD300AACC05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67133D7E-AD93-40EB-BBEC-A1B67747D5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="142">
   <si>
     <t>Leírás</t>
   </si>
@@ -1090,18 +1090,296 @@
       </rPr>
       <t>: 0.00% (0/15)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. tesztelés (2024. 12. 11.)
+Tesztelő: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ceglédi Zente Holló</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tesztkörnyezet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Operációs rendszer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Microsoft Windows [Version 10.0.19045.5131]
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Böngésző</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Brave: 1.73.91 Chromium: 131.0.6778.85 (Hivatalos verzió) (64 bites) 
+- Build: 79fcbad (foxhabits.com)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Eredmény</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 60.00% (9/15)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Partially</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 20.00% (3/15)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 20.00% (3/15)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skip</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 0.00% (0/15)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Partially
+Nem kapott értesítést a sikeres regisztrációról, vagy arról, hogy ellenőrző e-mailt küldtek. </t>
+  </si>
+  <si>
+    <t>Értesítést még fixálnunk kell, mert meghal tőle az oldal.</t>
+  </si>
+  <si>
+    <t>E-mail: kamuemail4@zente.org</t>
+  </si>
+  <si>
+    <t>Fail
+A linkre kattintottam 30 mp-en belül: "Érvénytelen vagy lejárt a visszaállítási link"</t>
+  </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>2-szer teszteltem, sajnos egyik esetben sem működött.</t>
+  </si>
+  <si>
+    <t>Fail
+Korábban részletezve</t>
+  </si>
+  <si>
+    <t>B101/1</t>
+  </si>
+  <si>
+    <t>B101/2</t>
+  </si>
+  <si>
+    <t>B102/1</t>
+  </si>
+  <si>
+    <t>B102/2</t>
+  </si>
+  <si>
+    <t>B102/3</t>
+  </si>
+  <si>
+    <t>B103</t>
+  </si>
+  <si>
+    <t>B104/1</t>
+  </si>
+  <si>
+    <t>B104/2</t>
+  </si>
+  <si>
+    <t>B104/3</t>
+  </si>
+  <si>
+    <t>B105</t>
+  </si>
+  <si>
+    <t>B106</t>
+  </si>
+  <si>
+    <t>B107</t>
+  </si>
+  <si>
+    <t>B108</t>
+  </si>
+  <si>
+    <t>B109</t>
+  </si>
+  <si>
+    <t>B110</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1171,6 +1449,21 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1505,7 +1798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1513,22 +1806,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1546,10 +1839,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1573,38 +1866,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2008,10 +2307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,18 +2327,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="23" t="s">
         <v>82</v>
       </c>
@@ -2308,18 +2607,18 @@
       <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="24" t="s">
         <v>116</v>
       </c>
@@ -2352,7 +2651,7 @@
       <c r="A16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -2378,7 +2677,7 @@
       <c r="A17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="2" t="s">
         <v>71</v>
       </c>
@@ -2399,7 +2698,7 @@
       <c r="A18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="30" t="s">
         <v>105</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2422,7 +2721,7 @@
       <c r="A19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="2" t="s">
         <v>61</v>
       </c>
@@ -2443,7 +2742,7 @@
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="27"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2487,7 +2786,7 @@
       <c r="A22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="30" t="s">
         <v>106</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -2510,7 +2809,7 @@
       <c r="A23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="2" t="s">
         <v>61</v>
       </c>
@@ -2531,7 +2830,7 @@
       <c r="A24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="27"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2663,7 +2962,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>103</v>
       </c>
@@ -2686,8 +2985,392 @@
         <v>78</v>
       </c>
     </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="32"/>
+      <c r="C37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="31"/>
+      <c r="C38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="31"/>
+      <c r="C42" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D14:F14"/>
@@ -2695,8 +3378,13 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B40:B42"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:F13 F15:F1048576">
+  <conditionalFormatting sqref="F2:F13 F15:F31 F33:F1048576">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Skip">
       <formula>NOT(ISERROR(SEARCH("Skip",F2)))</formula>
     </cfRule>

</xml_diff>